<commit_message>
done `day 2` lesson of the course
</commit_message>
<xml_diff>
--- a/ccna_track.xlsx
+++ b/ccna_track.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IMT\Desktop\ccna\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IMT\Desktop\CCNA_learning_track\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E033C257-EF56-4173-BFBD-BBA71B16B14F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD97183-F405-4FE9-9252-2D2F9D8F9254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{829FD34E-B036-4B25-82BC-10BAAFDCAD60}"/>
   </bookViews>
@@ -33,9 +33,96 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="22">
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>Types of Networks</t>
+  </si>
+  <si>
+    <t>Learning</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="9"/>
+        <rFont val="URWClassico"/>
+      </rPr>
+      <t>Computer Network</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="URWClassico"/>
+      </rPr>
+      <t>: is a digital telecommications networks that which allows nodes to share resources.</t>
+    </r>
+  </si>
+  <si>
+    <t>Dropped</t>
+  </si>
+  <si>
+    <t>Ongoing</t>
+  </si>
+  <si>
+    <t>Server &amp; Client</t>
+  </si>
+  <si>
+    <t>Switch &amp; Router</t>
+  </si>
+  <si>
+    <t>Firewall</t>
+  </si>
+  <si>
+    <t>Revising Needed</t>
+  </si>
+  <si>
+    <t>Revising Needed?</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>RJ-45(Registered Jack) &amp; SFP(Small Form-Factor Pluggable)</t>
+  </si>
+  <si>
+    <t>Interface &amp; Cables</t>
+  </si>
+  <si>
+    <t>UTP + STP+ Fiber Optic</t>
+  </si>
+  <si>
+    <t>Auto MDI-X</t>
+  </si>
+  <si>
+    <t>Straight-Through + Cross-Over Cables</t>
+  </si>
+  <si>
+    <t>Single-Mode + Multi-Mode Fiber Optics</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -43,16 +130,178 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="0.79998168889431442"/>
+      <name val="URWClassico"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="8" tint="0.79998168889431442"/>
+      <name val="URWClassico"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="7" tint="0.79998168889431442"/>
+      <name val="URWClassico"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="URWClassico"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="URWClassico"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="URWClassico"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="URWClassico"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color theme="7"/>
+      <name val="URWClassico"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color theme="5"/>
+      <name val="URWClassico"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color theme="9"/>
+      <name val="URWClassico"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color rgb="FFC00000"/>
+      <name val="URWClassico"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color theme="4"/>
+      <name val="URWClassico"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="URWClassico"/>
+    </font>
+    <font>
+      <i/>
+      <strike/>
+      <sz val="9"/>
+      <color theme="9"/>
+      <name val="URWClassico"/>
+    </font>
+    <font>
+      <i/>
+      <strike/>
+      <sz val="9"/>
+      <color theme="7"/>
+      <name val="URWClassico"/>
+    </font>
+    <font>
+      <i/>
+      <strike/>
+      <sz val="9"/>
+      <color theme="5"/>
+      <name val="URWClassico"/>
+    </font>
+    <font>
+      <i/>
+      <strike/>
+      <sz val="9"/>
+      <color rgb="FFC00000"/>
+      <name val="URWClassico"/>
+    </font>
+    <font>
+      <i/>
+      <strike/>
+      <sz val="9"/>
+      <color theme="4"/>
+      <name val="URWClassico"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="0.79998168889431442"/>
+      <name val="URWClassico"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFC00000"/>
+      <name val="URWClassico"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="9"/>
+      <name val="URWClassico"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="9"/>
+      <color rgb="FFC00000"/>
+      <name val="URWClassico"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="9"/>
+      <color theme="9"/>
+      <name val="URWClassico"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -60,18 +309,104 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFABAB"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -380,12 +715,279 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7B5293C-6BC6-48D8-A4A2-2B5C8B90AE98}">
-  <dimension ref="A1"/>
+  <dimension ref="F1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E2" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15.4" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="5" width="9.06640625" style="4"/>
+    <col min="6" max="6" width="50.265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" style="4" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="15.796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="12.9296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.796875" style="4" customWidth="1"/>
+    <col min="14" max="16384" width="9.06640625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="6:13" ht="61.5" x14ac:dyDescent="0.5">
+      <c r="M1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="6:13" x14ac:dyDescent="0.5">
+      <c r="F4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="L4" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="6:13" x14ac:dyDescent="0.5">
+      <c r="F5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="9">
+        <v>45161</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" s="19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="6:13" x14ac:dyDescent="0.5">
+      <c r="F6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="9">
+        <v>45161</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="L6" s="20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="6:13" x14ac:dyDescent="0.5">
+      <c r="F7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="9">
+        <v>45161</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="L7" s="22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="6:13" x14ac:dyDescent="0.5">
+      <c r="F8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="9">
+        <v>45161</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="L8" s="24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="6:13" x14ac:dyDescent="0.5">
+      <c r="F9" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="9">
+        <v>45161</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="25"/>
+      <c r="L9" s="6"/>
+    </row>
+    <row r="10" spans="6:13" x14ac:dyDescent="0.5">
+      <c r="F10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="9">
+        <v>45161</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="26"/>
+      <c r="L10" s="6"/>
+    </row>
+    <row r="11" spans="6:13" x14ac:dyDescent="0.5">
+      <c r="F11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="9">
+        <v>45161</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="L11" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="6:13" x14ac:dyDescent="0.5">
+      <c r="F12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="9">
+        <v>45161</v>
+      </c>
+      <c r="H12" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="L12" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="6:13" x14ac:dyDescent="0.5">
+      <c r="F13" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="9">
+        <v>45161</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="6:13" x14ac:dyDescent="0.5">
+      <c r="F14" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="9">
+        <v>45161</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="6:13" x14ac:dyDescent="0.5">
+      <c r="F15" s="8"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="6"/>
+    </row>
+    <row r="16" spans="6:13" x14ac:dyDescent="0.5">
+      <c r="F16" s="8"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" spans="6:9" x14ac:dyDescent="0.5">
+      <c r="F17" s="8"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" spans="6:9" x14ac:dyDescent="0.5">
+      <c r="F18" s="8"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" spans="6:9" x14ac:dyDescent="0.5">
+      <c r="F19" s="8"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+    </row>
+    <row r="20" spans="6:9" x14ac:dyDescent="0.5">
+      <c r="F20" s="8"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+    </row>
+    <row r="21" spans="6:9" x14ac:dyDescent="0.5">
+      <c r="F21" s="8"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+    </row>
+    <row r="22" spans="6:9" x14ac:dyDescent="0.5">
+      <c r="F22" s="8"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>